<commit_message>
commit harian, memulau SOP Kasir dan Sales
</commit_message>
<xml_diff>
--- a/Penomoran dokumen.xlsx
+++ b/Penomoran dokumen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="17100" windowHeight="9345"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="14040" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
     <t>Work Instruction</t>
   </si>
   <si>
-    <t>01/No.17 – Dok.03/2022</t>
+    <t>01/No.22 – Dok.02/2022</t>
   </si>
 </sst>
 </file>
@@ -233,12 +233,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -582,7 +585,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A7" sqref="A7:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,312 +595,312 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="9"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14" t="s">
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="6"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="7"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="9"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="9"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="9"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="13"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L19" t="s">
@@ -932,76 +935,76 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="13">
+      <c r="B23" s="14">
         <v>1</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13" t="s">
+      <c r="E23" s="14"/>
+      <c r="F23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13" t="s">
+      <c r="H23" s="14"/>
+      <c r="I23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="14">
         <v>2022</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
       <c r="L24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="4"/>
       <c r="F25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="4"/>
       <c r="I25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="L25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="M25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="L26" t="s">
         <v>23</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="L27" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
just harian, memulai kasir dan sales
</commit_message>
<xml_diff>
--- a/Penomoran dokumen.xlsx
+++ b/Penomoran dokumen.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>PENOMORAN DOKUMEN</t>
   </si>
@@ -93,7 +93,13 @@
     <t>Work Instruction</t>
   </si>
   <si>
-    <t>01/No.22 – Dok.02/2022</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>01/No.26 – Dok.03/VST/2022</t>
   </si>
 </sst>
 </file>
@@ -582,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D11"/>
+      <selection activeCell="I12" sqref="I12:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +728,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -813,7 +819,9 @@
       <c r="P11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
@@ -973,7 +981,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>12</v>
       </c>
@@ -1004,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L26" t="s">
         <v>23</v>
       </c>
@@ -1012,12 +1020,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L27" t="s">
         <v>24</v>
       </c>
       <c r="M27">
         <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>26</v>
+      </c>
+      <c r="M28">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
offline SOP jadi v 1.0
</commit_message>
<xml_diff>
--- a/Penomoran dokumen.xlsx
+++ b/Penomoran dokumen.xlsx
@@ -99,7 +99,7 @@
     <t>General</t>
   </si>
   <si>
-    <t>01/No.28 – Dok.04/VST/2022</t>
+    <t>03/No.32 – Dok.02/VST/2022</t>
   </si>
 </sst>
 </file>
@@ -248,9 +248,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -285,6 +282,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -601,314 +601,314 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="7"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="10"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="9"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="13"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="12"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15" t="s">
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="10"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="10"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="10"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="13"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="12"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L19" t="s">
@@ -943,40 +943,40 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="14">
+      <c r="B23" s="13">
         <v>1</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14" t="s">
+      <c r="E23" s="13"/>
+      <c r="F23" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14" t="s">
+      <c r="H23" s="13"/>
+      <c r="I23" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="13">
         <v>2022</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
       <c r="L24" t="s">
         <v>21</v>
       </c>
@@ -988,17 +988,17 @@
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="16"/>
       <c r="F25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1038,11 +1038,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:P3"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:H5"/>
-    <mergeCell ref="I4:L5"/>
-    <mergeCell ref="M4:P5"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A12:D16"/>
+    <mergeCell ref="E12:H16"/>
+    <mergeCell ref="I12:L16"/>
+    <mergeCell ref="M12:P16"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="I6:L6"/>
@@ -1051,19 +1059,11 @@
     <mergeCell ref="E7:H11"/>
     <mergeCell ref="I7:L11"/>
     <mergeCell ref="M7:P11"/>
-    <mergeCell ref="M12:P16"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A12:D16"/>
-    <mergeCell ref="E12:H16"/>
-    <mergeCell ref="I12:L16"/>
+    <mergeCell ref="A1:P3"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:H5"/>
+    <mergeCell ref="I4:L5"/>
+    <mergeCell ref="M4:P5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
25 Agustus 2022 10:04
</commit_message>
<xml_diff>
--- a/Penomoran dokumen.xlsx
+++ b/Penomoran dokumen.xlsx
@@ -105,7 +105,7 @@
     <t>ACCOUNTING</t>
   </si>
   <si>
-    <t>04/No.39 – Dok.02/VST/2022</t>
+    <t>04/No.40 – Dok.03/VST/2022</t>
   </si>
 </sst>
 </file>
@@ -254,6 +254,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -288,9 +291,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -597,7 +597,7 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:L16"/>
+      <selection activeCell="A7" sqref="A7:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,314 +608,314 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="9"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14" t="s">
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="7"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="9"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="9"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="9"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="13"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L19" t="s">
@@ -962,40 +962,40 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="13">
+      <c r="B23" s="14">
         <v>1</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13" t="s">
+      <c r="E23" s="14"/>
+      <c r="F23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13" t="s">
+      <c r="H23" s="14"/>
+      <c r="I23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="14">
         <v>2022</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
       <c r="L24" t="s">
         <v>21</v>
       </c>
@@ -1007,17 +1007,17 @@
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="4"/>
       <c r="F25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="G25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="16"/>
+      <c r="H25" s="4"/>
       <c r="I25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1057,11 +1057,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A12:D16"/>
-    <mergeCell ref="E12:H16"/>
-    <mergeCell ref="I12:L16"/>
+    <mergeCell ref="A1:P3"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:H5"/>
+    <mergeCell ref="I4:L5"/>
+    <mergeCell ref="M4:P5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="A7:D11"/>
+    <mergeCell ref="E7:H11"/>
+    <mergeCell ref="I7:L11"/>
+    <mergeCell ref="M7:P11"/>
     <mergeCell ref="M12:P16"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
@@ -1070,19 +1078,11 @@
     <mergeCell ref="G23:H24"/>
     <mergeCell ref="I23:I24"/>
     <mergeCell ref="J23:J24"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="A7:D11"/>
-    <mergeCell ref="E7:H11"/>
-    <mergeCell ref="I7:L11"/>
-    <mergeCell ref="M7:P11"/>
-    <mergeCell ref="A1:P3"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:H5"/>
-    <mergeCell ref="I4:L5"/>
-    <mergeCell ref="M4:P5"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A12:D16"/>
+    <mergeCell ref="E12:H16"/>
+    <mergeCell ref="I12:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>